<commit_message>
New EDT2 version implemented. Paramter adaptive added. New emotion added to the dict.
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\EDT\data_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/EDT/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23383295-4947-42DF-B39A-05A347E67957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F74954B-1D60-7045-A436-023303FF9235}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="27495" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>key</t>
   </si>
@@ -334,13 +334,28 @@
   </si>
   <si>
     <t>Uw score</t>
+  </si>
+  <si>
+    <t>FEARFUL</t>
+  </si>
+  <si>
+    <t>ängstlicher</t>
+  </si>
+  <si>
+    <t>more fearful</t>
+  </si>
+  <si>
+    <t>angstig</t>
+  </si>
+  <si>
+    <t>более пугающей</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -373,6 +388,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Textkörper)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -394,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -407,6 +427,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -782,20 +803,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="112.140625" customWidth="1"/>
-    <col min="5" max="5" width="50.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="112.1640625" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="50.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +834,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -829,7 +851,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="157.5">
+    <row r="3" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -846,7 +868,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -863,7 +885,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -880,7 +902,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75">
+    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -897,7 +919,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -914,7 +936,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -931,7 +953,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -948,7 +970,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -965,7 +987,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -982,7 +1004,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1021,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1016,139 +1038,156 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" t="s">
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>75</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>81</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>83</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>77</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>79</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>80</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated dict, Readme file and added adaptive parameter to the file descriptions.
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/EDT/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F74954B-1D60-7045-A436-023303FF9235}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC6F8C-5B73-FB43-B27B-8A22E8F64E84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>Dein Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
   </si>
   <si>
-    <t>Bitte höre dir die folgenden Musikausschnitte an und entscheide, welche sich **{{emotion}}**  anhörte. Wähle 1 für den Ausschnitt vor dem Summton und 2 für den Ausschnitt danach.</t>
-  </si>
-  <si>
     <t>Bitte eine Option auswählen.</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
   </si>
   <si>
     <t>Your browser doesn't support audio. This test won't work without audio, sorry!</t>
-  </si>
-  <si>
-    <t>Please listen to the following clips and select which one sounds **{{emotion}}** to you. Select 1 for the clip heard before the buzzer, or 2 for the clip heard after the buzzer.</t>
   </si>
   <si>
     <t>Please select one option.</t>
@@ -349,6 +343,12 @@
   </si>
   <si>
     <t>более пугающей</t>
+  </si>
+  <si>
+    <t>Bitte höre dir die folgenden Musikausschnitte an und entscheide, welche sich **{{emotion}}**  anhörte. Wähle 1 für den Ausschnitt vor dem Piepton und 2 für den Ausschnitt danach.</t>
+  </si>
+  <si>
+    <t>Please listen to the following clips and select which one sounds **{{emotion}}** to you. Select 1 for the clip heard before the beep, or 2 for the clip heard after the beep.</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -805,14 +805,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="112.1640625" customWidth="1"/>
+    <col min="2" max="2" width="75.1640625" customWidth="1"/>
+    <col min="3" max="3" width="101" customWidth="1"/>
     <col min="4" max="4" width="52.33203125" customWidth="1"/>
     <col min="5" max="5" width="50.1640625" customWidth="1"/>
   </cols>
@@ -831,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -839,16 +840,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="153" x14ac:dyDescent="0.2">
@@ -859,13 +860,13 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -876,13 +877,13 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -893,13 +894,13 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -907,16 +908,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -924,16 +925,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -941,16 +942,16 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -958,16 +959,16 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -975,16 +976,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -992,16 +993,16 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1009,16 +1010,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1026,33 +1027,33 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
         <v>104</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
         <v>105</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1060,16 +1061,16 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1077,16 +1078,16 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1094,16 +1095,16 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1111,16 +1112,16 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1128,16 +1129,16 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -1145,16 +1146,16 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1162,16 +1163,16 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1179,16 +1180,16 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added training to the EDT using the parameter take_training. Dictionnary was adapted accordingly.
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/EDT/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC6F8C-5B73-FB43-B27B-8A22E8F64E84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB33EA7A-DABE-E74B-8894-5F03C93A2EBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
   <si>
     <t>key</t>
   </si>
@@ -349,13 +349,146 @@
   </si>
   <si>
     <t>Please listen to the following clips and select which one sounds **{{emotion}}** to you. Select 1 for the clip heard before the beep, or 2 for the clip heard after the beep.</t>
+  </si>
+  <si>
+    <t>GOBACK</t>
+  </si>
+  <si>
+    <t>Gehe zurück</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS</t>
+  </si>
+  <si>
+    <t>MAIN_INTRO</t>
+  </si>
+  <si>
+    <t>SAMPLE1a</t>
+  </si>
+  <si>
+    <t>For each trial, the two melodies you hear will be identical except that they will each be intended to communicate a different expression. Listen to the following clip by clicking the play button, and decide which of the two melodies sounds **happier** to you. \\ Here, the performer intended to convey a happy expression in the melody heard before the beep, and a sad expression in the melody heard after the beep, so the correct answer would have been clip 1. Feel free to listen again before moving on.</t>
+  </si>
+  <si>
+    <t>TRANSITION</t>
+  </si>
+  <si>
+    <t>PRACTICE1</t>
+  </si>
+  <si>
+    <t>PRACTICE2</t>
+  </si>
+  <si>
+    <t>INCORRECT</t>
+  </si>
+  <si>
+    <t>CORRECT</t>
+  </si>
+  <si>
+    <t>Incorrect.</t>
+  </si>
+  <si>
+    <t>Falsch.</t>
+  </si>
+  <si>
+    <t>Richtig!</t>
+  </si>
+  <si>
+    <t>Correct!</t>
+  </si>
+  <si>
+    <t>Nun geht es mit dem Haupttest los, in dem deine Ergebnisse gespeichert werden. \\ Ab jetzt bekommst du keine Rückmeldung mehr. Viel Erfolg!</t>
+  </si>
+  <si>
+    <t>You are about to start the main test, where your results will be recorded. \\ You won't receive any feedback after individual questions. Good luck!</t>
+  </si>
+  <si>
+    <t>Welcome to the Musical Emotion Discrimination Training. \\  You will be asked to listen to pairs of pre-recorded melodies which were performed with the intention of expressing one of five emotional categories: anger, fear, happiness, sadness or tenderness. Your task is to discriminate between the expressions communicated in each clip. \\ First, you’ll hear some examples and do a few practice questions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time for some practice: \\ **Practice question 1:** \\ Please listen to the following clips and select which one sounds **angrier** to you. Select 1 for the clip heard before the beep, or 2 for the clip heard after the beep. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">**{{feedback}}** \\ Press ‘Go back’ to read the instructions and do the practice questions again, or press ‘Continue’ to continue to the main test. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **{{feedback}}** \\ Here’s another example. \\ **Practice question 2:** \\Please listen to the following clips and select which one sounds **sadder** to you. Select 1 for the clip heard before the beep, or 2 for the clip heard after the beep. </t>
+  </si>
+  <si>
+    <t>Willkommen zur Emotionen-Unterscheidungstest Übung. \\ Du wirst gleich gebeten dir zwei aufgezeichnete Melodiepaare anzuhören, die mit der Absicht aufgenommen wurden, eine von fünf bestimmten Emotionen auszudrücken: Wut, Angst, Freude, Trauer und Zärtlichkeit. Deine Aufgabe ist es die Aufnahme zu benennen, die die gesuchte Emotion zeigt. \\ Zuerst wirst du Beispiele hören und dann ein paar Übungsaufgaben machen.</t>
+  </si>
+  <si>
+    <t>Добро пожаловать на тренинг по распознаванию музыкальных эмоций.\\ Вам будет предложено прослушать пары заранее записанных мелодий, которые были исполнены с намерением выразить одну из пяти эмоциональных категорий: гнев, страх, счастье, печаль или нежность. Ваша задача - различать выражения, передаваемые в каждом клипе. \\ Сначала вы услышите несколько примеров и зададите несколько практических вопросов.</t>
+  </si>
+  <si>
+    <t>Welkom bij de training Musical Emotion Discrimination. \\ U wordt gevraagd naar paren vooraf opgenomen melodieën te luisteren die zijn uitgevoerd met de bedoeling een van de vijf emotionele categorieën uit te drukken: woede, angst, geluk, verdriet of tederheid. Het is jouw taak om onderscheid te maken tussen de uitdrukkingen die in elke clip worden gecommuniceerd. \\ Eerst hoor je enkele voorbeelden en doe je een paar oefenvragen.</t>
+  </si>
+  <si>
+    <t>Ga terug</t>
+  </si>
+  <si>
+    <t>Вернитесь назад</t>
+  </si>
+  <si>
+    <t>Bei jedem Durchgang sind die beiden Melodien, die du hörst, identisch, mit der Ausnahme, dass sie jeweils einen anderen Ausdruck vermitteln sollen. Hör dir den folgenden Clip an, indem du auf die Wiedergabetaste klickst, und entscheide, welche der beiden Melodien für dich **fröhlicher** klingt. \\
+In diesem Beispiel wollte der Musiker einen fröhlichen Ausdruck in der Melodie vermitteln, die vor dem Piepton zu hören war, und einen traurigen Ausdruck in der Melodie, die nach dem Piepton zu hören war. Die richtige Antwort wäre also Nummer 1. Du kannst gerne noch einmal zuhören, bevor du fortfährst.</t>
+  </si>
+  <si>
+    <t>Для каждого испытания две мелодии, которые вы слышите, будут идентичны, за исключением того, что каждая из них предназначена для передачи разного выражения. Прослушайте следующий клип, нажав кнопку воспроизведения, и решите, какая из двух мелодий вам нравится больше. \\ Здесь исполнитель намеревался передать счастливое выражение в мелодии, слышимой перед звуковым сигналом, и грустное выражение в мелодии, слышимой после звукового сигнала, поэтому правильным ответом был бы клип 1. Не стесняйтесь послушать еще раз, прежде чем двигаться дальше.</t>
+  </si>
+  <si>
+    <t>Voor elke proef zijn de twee melodieën die u hoort identiek, behalve dat ze elk bedoeld zijn om een andere uitdrukking over te brengen. Luister naar de volgende clip door op de afspeelknop te klikken en bepaal welke van de twee melodieën u gelukkiger in de oren klinkt. \\ Hier wilde de artiest een vrolijke uitdrukking overbrengen in de melodie die vóór de piep hoorde, en een droevige uitdrukking in de melodie die na de piep hoorde, dus het juiste antwoord zou clip 1 zijn geweest. Voel je vrij om nog een keer te luisteren voordat je verder gaat.</t>
+  </si>
+  <si>
+    <t>Zeit zum Üben: \\ **Übungsfrage 1:** \\ Bitte höre dir die folgenden Clips an und wähle aus, welcher für dich **wütender** klingt. Wähle 1 für den Clip, der vor dem Piepton zu hören ist, oder 2 für den Clip, der nach dem Piepton zu hören ist.</t>
+  </si>
+  <si>
+    <t>Время для практики: \\ **Практический вопрос 1.** \\  Прослушайте следующие клипы и выберите, какой из них звучит для вас **злее**. Выберите 1 для клипа, который слышен до сигнала, или 2 для клипа, который слышен после сигнала.</t>
+  </si>
+  <si>
+    <t>Tijd voor wat oefening: \\ **Oefenvraag 1:** \\  Luister alsjeblieft naar de volgende clips en selecteer welke je **bozer** vindt. Selecteer 1 voor de clip die u hoort vóór de pieptoon, of 2 voor de clip die u hoort na de pieptoon.</t>
+  </si>
+  <si>
+    <t>Niet correct.</t>
+  </si>
+  <si>
+    <t>Неправильно.</t>
+  </si>
+  <si>
+    <t>Правильный!</t>
+  </si>
+  <si>
+    <t>U staat op het punt de hoofdtest te starten, waar uw resultaten worden geregistreerd. \\ U ontvangt geen feedback na individuele vragen. Succes!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вы собираетесь начать основной тест, на котором будут записаны ваши результаты. \\ Вы не получите никаких отзывов после индивидуальных вопросов. Удачи! </t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Klicke auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicke auf 'Weiter', um zum  Haupttest zu gelangen.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Другой пример. \\ **Практический вопрос 2:** \\ Пожалуйста, послушайте следующие клипы и выберите, какой из них звучит **печальнее** для вас. Выберите 1 для клипа, который слышен до сигнала, или 2 для клипа, который слышен после сигнала.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Нажмите «Вернуться», чтобы прочитать инструкции и снова ответить на практические вопросы, или нажмите «Продолжить», чтобы перейти к основному тесту.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Druk op ‘Ga terug’ om de instructies te lezen en de oefenvragen opnieuw uit te voeren, of druk op ‘Doorgaan’ om door te gaan naar de hoofdtest.</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Hier is nog een voorbeeld. \\ **Oefenvraag 2:** \\ Luister naar de volgende clips en selecteer welke u **droeviger** vindt. Selecteer 1 voor de clip die u hoort vóór de pieptoon, of 2 voor de clip die u hoort na de pieptoon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**{{feedback}}** \\ Hier ist ein weiteres Beispiel. \\ **Übungsfrage 2:** \\ Bitte höre dir die folgenden Clips an und wähle aus, welcher für dich **trauriger** klingt. Wähle 1 für den Clip, der vor dem Piepton zu hören ist, oder 2 für den Clip, der nach dem Piepton zu hören ist. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -374,6 +507,7 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -392,6 +526,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri (Textkörper)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,20 +555,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -458,7 +597,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -803,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -835,7 +974,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -848,11 +987,11 @@
       <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -865,11 +1004,11 @@
       <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -882,11 +1021,11 @@
       <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -899,11 +1038,11 @@
       <c r="D5" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -916,7 +1055,7 @@
       <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>87</v>
       </c>
     </row>
@@ -933,7 +1072,7 @@
       <c r="D7" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -950,7 +1089,7 @@
       <c r="D8" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -967,7 +1106,7 @@
       <c r="D9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -984,7 +1123,7 @@
       <c r="D10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1049,7 +1188,7 @@
       <c r="C14" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E14" t="s">
@@ -1073,7 +1212,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1225,7 @@
       <c r="D16" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="6" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1120,7 +1259,7 @@
       <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1141,7 +1280,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1154,7 +1293,7 @@
       <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="6" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1190,6 +1329,159 @@
       </c>
       <c r="E22" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" t="s">
+        <v>143</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New order of the sample pages when take_traing = TRUE. Russian translation added.
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/EDT/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB33EA7A-DABE-E74B-8894-5F03C93A2EBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC9463-6DB0-B042-A365-CB51AF6690B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="19160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36240" yWindow="-2920" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="158">
   <si>
     <t>key</t>
   </si>
@@ -369,9 +369,6 @@
     <t>SAMPLE1a</t>
   </si>
   <si>
-    <t>For each trial, the two melodies you hear will be identical except that they will each be intended to communicate a different expression. Listen to the following clip by clicking the play button, and decide which of the two melodies sounds **happier** to you. \\ Here, the performer intended to convey a happy expression in the melody heard before the beep, and a sad expression in the melody heard after the beep, so the correct answer would have been clip 1. Feel free to listen again before moving on.</t>
-  </si>
-  <si>
     <t>TRANSITION</t>
   </si>
   <si>
@@ -420,9 +417,6 @@
     <t>Willkommen zur Emotionen-Unterscheidungstest Übung. \\ Du wirst gleich gebeten dir zwei aufgezeichnete Melodiepaare anzuhören, die mit der Absicht aufgenommen wurden, eine von fünf bestimmten Emotionen auszudrücken: Wut, Angst, Freude, Trauer und Zärtlichkeit. Deine Aufgabe ist es die Aufnahme zu benennen, die die gesuchte Emotion zeigt. \\ Zuerst wirst du Beispiele hören und dann ein paar Übungsaufgaben machen.</t>
   </si>
   <si>
-    <t>Добро пожаловать на тренинг по распознаванию музыкальных эмоций.\\ Вам будет предложено прослушать пары заранее записанных мелодий, которые были исполнены с намерением выразить одну из пяти эмоциональных категорий: гнев, страх, счастье, печаль или нежность. Ваша задача - различать выражения, передаваемые в каждом клипе. \\ Сначала вы услышите несколько примеров и зададите несколько практических вопросов.</t>
-  </si>
-  <si>
     <t>Welkom bij de training Musical Emotion Discrimination. \\ U wordt gevraagd naar paren vooraf opgenomen melodieën te luisteren die zijn uitgevoerd met de bedoeling een van de vijf emotionele categorieën uit te drukken: woede, angst, geluk, verdriet of tederheid. Het is jouw taak om onderscheid te maken tussen de uitdrukkingen die in elke clip worden gecommuniceerd. \\ Eerst hoor je enkele voorbeelden en doe je een paar oefenvragen.</t>
   </si>
   <si>
@@ -432,34 +426,15 @@
     <t>Вернитесь назад</t>
   </si>
   <si>
-    <t>Bei jedem Durchgang sind die beiden Melodien, die du hörst, identisch, mit der Ausnahme, dass sie jeweils einen anderen Ausdruck vermitteln sollen. Hör dir den folgenden Clip an, indem du auf die Wiedergabetaste klickst, und entscheide, welche der beiden Melodien für dich **fröhlicher** klingt. \\
-In diesem Beispiel wollte der Musiker einen fröhlichen Ausdruck in der Melodie vermitteln, die vor dem Piepton zu hören war, und einen traurigen Ausdruck in der Melodie, die nach dem Piepton zu hören war. Die richtige Antwort wäre also Nummer 1. Du kannst gerne noch einmal zuhören, bevor du fortfährst.</t>
-  </si>
-  <si>
-    <t>Для каждого испытания две мелодии, которые вы слышите, будут идентичны, за исключением того, что каждая из них предназначена для передачи разного выражения. Прослушайте следующий клип, нажав кнопку воспроизведения, и решите, какая из двух мелодий вам нравится больше. \\ Здесь исполнитель намеревался передать счастливое выражение в мелодии, слышимой перед звуковым сигналом, и грустное выражение в мелодии, слышимой после звукового сигнала, поэтому правильным ответом был бы клип 1. Не стесняйтесь послушать еще раз, прежде чем двигаться дальше.</t>
-  </si>
-  <si>
-    <t>Voor elke proef zijn de twee melodieën die u hoort identiek, behalve dat ze elk bedoeld zijn om een andere uitdrukking over te brengen. Luister naar de volgende clip door op de afspeelknop te klikken en bepaal welke van de twee melodieën u gelukkiger in de oren klinkt. \\ Hier wilde de artiest een vrolijke uitdrukking overbrengen in de melodie die vóór de piep hoorde, en een droevige uitdrukking in de melodie die na de piep hoorde, dus het juiste antwoord zou clip 1 zijn geweest. Voel je vrij om nog een keer te luisteren voordat je verder gaat.</t>
-  </si>
-  <si>
     <t>Zeit zum Üben: \\ **Übungsfrage 1:** \\ Bitte höre dir die folgenden Clips an und wähle aus, welcher für dich **wütender** klingt. Wähle 1 für den Clip, der vor dem Piepton zu hören ist, oder 2 für den Clip, der nach dem Piepton zu hören ist.</t>
   </si>
   <si>
-    <t>Время для практики: \\ **Практический вопрос 1.** \\  Прослушайте следующие клипы и выберите, какой из них звучит для вас **злее**. Выберите 1 для клипа, который слышен до сигнала, или 2 для клипа, который слышен после сигнала.</t>
-  </si>
-  <si>
     <t>Tijd voor wat oefening: \\ **Oefenvraag 1:** \\  Luister alsjeblieft naar de volgende clips en selecteer welke je **bozer** vindt. Selecteer 1 voor de clip die u hoort vóór de pieptoon, of 2 voor de clip die u hoort na de pieptoon.</t>
   </si>
   <si>
     <t>Niet correct.</t>
   </si>
   <si>
-    <t>Неправильно.</t>
-  </si>
-  <si>
-    <t>Правильный!</t>
-  </si>
-  <si>
     <t>U staat op het punt de hoofdtest te starten, waar uw resultaten worden geregistreerd. \\ U ontvangt geen feedback na individuele vragen. Succes!</t>
   </si>
   <si>
@@ -469,12 +444,6 @@
     <t>**{{feedback}}** \\ Klicke auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicke auf 'Weiter', um zum  Haupttest zu gelangen.</t>
   </si>
   <si>
-    <t>**{{feedback}}** \\ Другой пример. \\ **Практический вопрос 2:** \\ Пожалуйста, послушайте следующие клипы и выберите, какой из них звучит **печальнее** для вас. Выберите 1 для клипа, который слышен до сигнала, или 2 для клипа, который слышен после сигнала.</t>
-  </si>
-  <si>
-    <t>**{{feedback}}** \\ Нажмите «Вернуться», чтобы прочитать инструкции и снова ответить на практические вопросы, или нажмите «Продолжить», чтобы перейти к основному тесту.</t>
-  </si>
-  <si>
     <t>**{{feedback}}** \\ Druk op ‘Ga terug’ om de instructies te lezen en de oefenvragen opnieuw uit te voeren, of druk op ‘Doorgaan’ om door te gaan naar de hoofdtest.</t>
   </si>
   <si>
@@ -482,6 +451,53 @@
   </si>
   <si>
     <t xml:space="preserve">**{{feedback}}** \\ Hier ist ein weiteres Beispiel. \\ **Übungsfrage 2:** \\ Bitte höre dir die folgenden Clips an und wähle aus, welcher für dich **trauriger** klingt. Wähle 1 für den Clip, der vor dem Piepton zu hören ist, oder 2 für den Clip, der nach dem Piepton zu hören ist. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добро пожаловать! // Предлагаем вам выполнить тест на способность определять эмоции в музыке. Вам будет предложено прослушать пары мелодий, в каждой из которых исполнитель стремился передает одну из пяти эмоций: злость, страх, радость, грусть или нежность. Ваша задача – определить эмоцию каждой мелодии. // Для начала прослушайте несколько примеров и выполните тренировочные задания. </t>
+  </si>
+  <si>
+    <t>SAMPLE1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei jedem Durchgang sind die beiden Melodien, die du hörst, identisch, mit der Ausnahme, dass sie jeweils einen anderen Ausdruck vermitteln sollen. Hör dir den folgenden Clip an, indem du auf die Wiedergabetaste klickst, und entscheide, welche der beiden Melodien für dich **fröhlicher** klingt.
+</t>
+  </si>
+  <si>
+    <t>In diesem Beispiel wollte der Musiker einen fröhlichen Ausdruck in der Melodie vermitteln, die vor dem Piepton zu hören war, und einen traurigen Ausdruck in der Melodie, die nach dem Piepton zu hören war. Die richtige Antwort wäre also Nummer 1. Du kannst gerne noch einmal zuhören, bevor du fortfährst.</t>
+  </si>
+  <si>
+    <t>For each trial, the two melodies you hear will be identical except that they will each be intended to communicate a different expression. Listen to the following clip by clicking the play button, and decide which of the two melodies sounds **happier** to you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Here, the performer intended to convey a happy expression in the melody heard before the beep, and a sad expression in the melody heard after the beep, so the correct answer would have been clip 1. Feel free to listen again before moving on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В каждом задании вы услышите две похожих мелодии, которые будут отличаться только тем, какую эмоцию они передают. Чтобы прослушать мелодии, нажмите на кнопку воспроизведения, а затем выберите, какая из мелодий звучит **радостнее**. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> В этом примере исполнитель стремился передать радость в мелодии, которая прозвучала до звукового сигнала. В мелодии, которая прозвучала после звукового сигнала, исполнитель стремился передать грусть. Следовательно, правильным ответом будет мелодия 1. Вы можете прослушать мелодии повторно, прежде чем продолжить. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voor elke proef zijn de twee melodieën die u hoort identiek, behalve dat ze elk bedoeld zijn om een andere uitdrukking over te brengen. Luister naar de volgende clip door op de afspeelknop te klikken en bepaal welke van de twee melodieën u gelukkiger in de oren klinkt. </t>
+  </si>
+  <si>
+    <t>Hier wilde de artiest een vrolijke uitdrukking overbrengen in de melodie die vóór de piep hoorde, en een droevige uitdrukking in de melodie die na de piep hoorde, dus het juiste antwoord zou clip 1 zijn geweest. Voel je vrij om nog een keer te luisteren voordat je verder gaat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тренировочные задания: \\
+Тренировка 1: \\ Пожалуйста, прослушайте следующие мелодии и выберите, какая из них звучит **злее**. Нажмите 1, чтобы выбрать мелодию, прозвучавшую до звукового сигнала. Нажмите 2, чтобы выбрать мелодию, прозвучавшую после звукового сигнала. </t>
+  </si>
+  <si>
+    <t>Верно!</t>
+  </si>
+  <si>
+    <t>Неверно.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**{{feedback}}** \\ Еще один пример:  \\ **Тренировка 2:** \\ Пожалуйста, прослушайте следующие мелодии и выберите, какая из мелодий звучит **грустнее**. Нажмите 1, чтобы выбрать мелодию, прозвучавшую до звукового сигнала. Нажмите 2, чтобы выбрать мелодию, прозвучавшую после звукового сигнала. </t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Нажмите «Назад», чтобы вернуться к инструкциям и пройти тренировку еще раз. Нажмите «Продолжить», чтобы начать тест.</t>
   </si>
 </sst>
 </file>
@@ -942,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1342,10 +1358,10 @@
         <v>111</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1353,135 +1369,152 @@
         <v>112</v>
       </c>
       <c r="B24" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" t="s">
         <v>131</v>
       </c>
-      <c r="C24" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>136</v>
+      <c r="B25" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="D26" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" t="s">
-        <v>148</v>
+        <v>116</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>142</v>
+        <v>157</v>
+      </c>
+      <c r="E29" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
         <v>120</v>
       </c>
-      <c r="B30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" t="s">
-        <v>124</v>
-      </c>
       <c r="D30" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" t="s">
-        <v>124</v>
+        <v>155</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>113</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" t="s">
         <v>125</v>
       </c>
-      <c r="C31" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" t="s">
-        <v>146</v>
-      </c>
-      <c r="E31" t="s">
-        <v>145</v>
+      <c r="D32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor change in Russian translation.
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/EDT/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC9463-6DB0-B042-A365-CB51AF6690B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B69046A-B0C2-AF46-AAA0-3690E838BBAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36240" yWindow="-2920" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,9 +438,6 @@
     <t>U staat op het punt de hoofdtest te starten, waar uw resultaten worden geregistreerd. \\ U ontvangt geen feedback na individuele vragen. Succes!</t>
   </si>
   <si>
-    <t xml:space="preserve">Вы собираетесь начать основной тест, на котором будут записаны ваши результаты. \\ Вы не получите никаких отзывов после индивидуальных вопросов. Удачи! </t>
-  </si>
-  <si>
     <t>**{{feedback}}** \\ Klicke auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicke auf 'Weiter', um zum  Haupttest zu gelangen.</t>
   </si>
   <si>
@@ -498,6 +495,9 @@
   </si>
   <si>
     <t>**{{feedback}}** \\ Нажмите «Назад», чтобы вернуться к инструкциям и пройти тренировку еще раз. Нажмите «Продолжить», чтобы начать тест.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сейчас начнется основной тест, во время которого ваши ответы будут записаны. \\ Вы не будете получать обратной связи по каждому заданию. Желаем удачи! </t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -960,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1375,7 +1375,7 @@
         <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
         <v>131</v>
@@ -1386,33 +1386,33 @@
         <v>114</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="96" x14ac:dyDescent="0.2">
@@ -1426,7 +1426,7 @@
         <v>127</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
         <v>135</v>
@@ -1437,16 +1437,16 @@
         <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1454,16 +1454,16 @@
         <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
         <v>128</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1477,7 +1477,7 @@
         <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>136</v>
@@ -1494,7 +1494,7 @@
         <v>123</v>
       </c>
       <c r="D31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E31" t="s">
         <v>123</v>
@@ -1511,7 +1511,7 @@
         <v>125</v>
       </c>
       <c r="D32" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="E32" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Fixed non-adaptive test, new EDT2 item bank
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickruth/Documents/LongGold/EDT/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B69046A-B0C2-AF46-AAA0-3690E838BBAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2B5DC-4F20-AE41-9C79-ACC78A0B605B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36240" yWindow="-2920" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="170">
   <si>
     <t>key</t>
   </si>
@@ -498,6 +498,42 @@
   </si>
   <si>
     <t xml:space="preserve">Сейчас начнется основной тест, во время которого ваши ответы будут записаны. \\ Вы не будете получать обратной связи по каждому заданию. Желаем удачи! </t>
+  </si>
+  <si>
+    <t>ANGER</t>
+  </si>
+  <si>
+    <t>HAPPY</t>
+  </si>
+  <si>
+    <t>SAD</t>
+  </si>
+  <si>
+    <t>FEAR</t>
+  </si>
+  <si>
+    <t>am wütendsten</t>
+  </si>
+  <si>
+    <t>am fröhlichsten</t>
+  </si>
+  <si>
+    <t>am traurigsten</t>
+  </si>
+  <si>
+    <t>am ängstlichsten</t>
+  </si>
+  <si>
+    <t>happiest</t>
+  </si>
+  <si>
+    <t>angriest</t>
+  </si>
+  <si>
+    <t>saddest</t>
+  </si>
+  <si>
+    <t>most fearful</t>
   </si>
 </sst>
 </file>
@@ -639,7 +675,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -958,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1517,6 +1553,74 @@
         <v>137</v>
       </c>
     </row>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added formal German (de_f)
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\EDT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C49006-242B-46B5-B89A-125CA1A080EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1056DFA-A176-4A7D-98DC-851D6D011158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="253">
   <si>
     <t>key</t>
   </si>
@@ -726,6 +726,64 @@
   </si>
   <si>
     <t>**{{feedback}}** \\ **Pregunta de práctica 2** \\ Escucha los siguientes fragmentos y selecciona el que te suene **más triste**. \\ Selecciona 1 para el fragmento que escuchaste antes de la señal acústica , o 2 para el fragmento escuchado después de la señal acústica.</t>
+  </si>
+  <si>
+    <t>DE_F</t>
+  </si>
+  <si>
+    <t>Sie werden zwei Melodien hintereinander hören, die sich in dem emotionalen Ausdruck unterscheiden, mit dem sie gespielt wurden.   Ihre Aufgabe ist es, diejenige Melodie auszuwählen, die Ihrer Meinung nach, dem emotionalen Ausdruck in der Fragestellung am nächsten kommt. \\  Bitte hören Sie sich beide Melodien immer ganz an, bevor Sie Ihre Antwort auswählen. Fallst Sie sich nicht sicher sind, wählen Sie einfach Ihre beste Vermutung aus.  Antworten können sich wiederholen, und Sie können mehrmals hintereinander dieselbe Antwortmöglichkeit wählen.</t>
+  </si>
+  <si>
+    <t>Der Browser unterstützt kein Audio. Dieser Test funktioniert nicht ohne Audio, sorry!</t>
+  </si>
+  <si>
+    <t>Bitte hören Sie sich die folgenden Musikausschnitte an und entscheide Sie, welche sich **{{emotion}}**  anhörte. Wählen Sie 1 für den Ausschnitt vor dem Piepton und 2 für den Ausschnitt danach.</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie eine Option aus.</t>
+  </si>
+  <si>
+    <t>Sie haben **{{accuracy}} %** der Emotionen richtig erkannt.</t>
+  </si>
+  <si>
+    <t>Bitte geben Sie Ihre ID ein</t>
+  </si>
+  <si>
+    <t>Die ID ist leider ungültig. Bitte versuchen Sie es noch mal.</t>
+  </si>
+  <si>
+    <t>Sie haben den Emotionen-Unterscheidungstest erfolgreich beendet.</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} von {{num_question}} Fragen richtig beantwortet.</t>
+  </si>
+  <si>
+    <t>Ihr Testergebnis</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Willkommen zur Emotionen-Unterscheidungstest Übung&lt;/h4&gt;  Sie werden gleich gebeten, sich zwei aufgezeichnete Melodiepaare anzuhören, die mit der Absicht aufgenommen wurden, eine von fünf bestimmten Emotionen auszudrücken: Wut, Angst, Freude, Trauer und Zärtlichkeit. Ihre Aufgabe ist es, diejenige Aufnahme zu benennen, die die gesuchte Emotion zeigt. \\ Zuerst werden Sie Beispiele hören und dann ein paar Übungsaufgaben machen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei jedem Durchgang sind die beiden Melodien, die Sie hören, musikalisch identisch, aber sie sollen jeweils einen anderen Ausdruck vermitteln. Hör Sie sich den folgenden Clip an, indem Sie auf die Wiedergabetaste klicken, und entscheiden Sie, welche der beiden Melodien für Sie **fröhlicher** klingt.
+</t>
+  </si>
+  <si>
+    <t>In diesem Beispiel wollte der Musiker einen fröhlichen Ausdruck in der Melodie vermitteln, die vor dem Piepton zu hören war, und einen traurigen Ausdruck in der Melodie, die nach dem Piepton zu hören war. Die richtige Antwort wäre also Nummer 1. Sie können gerne noch einmal zuhören, bevor Sie fortfahren.</t>
+  </si>
+  <si>
+    <t>**Übungsfrage 1** \\ Bitte höre Sie sich die folgenden Clips an und wählen Sie aus, welcher für Sie **wütender** klingt. \\ Wählen Sie 1 für den Clip, der vor dem Piepton zu hören ist, oder 2 für den Clip, der nach dem Piepton zu hören ist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**{{feedback}}** \\ **Übungsfrage 2** \\ Bitte hören Sie sich die folgenden Clips an und wähle Sie aus, welcher für Sie **trauriger** klingt. \\ Wählen Sie 1 für den Clip, der vor dem Piepton zu hören ist, oder 2 für den Clip, der nach dem Piepton zu hören ist. </t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ Klicken Sie auf 'Zurück', um die Anweisungen erneut zu lesen und die Beispiele erneut zu versuchen, oder klicken Sie auf 'Weiter', um zum  Haupttest zu gelangen.</t>
+  </si>
+  <si>
+    <t>Zurück</t>
+  </si>
+  <si>
+    <t>Nun geht es mit dem Haupttest los, in dem Ihre Ergebnisse gespeichert werden. \\ Ab jetzt bekommen Sie keine Rückmeldung mehr. Viel Erfolg!</t>
   </si>
 </sst>
 </file>
@@ -846,13 +904,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>225926</xdr:rowOff>
@@ -1200,25 +1258,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E29" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="55" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="81.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="3" width="55" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="2" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="81.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1226,22 +1284,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1249,22 +1310,25 @@
         <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="270">
+    <row r="3" spans="1:8" ht="270">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1272,22 +1336,25 @@
         <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.5">
+    <row r="4" spans="1:8" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1295,22 +1362,25 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1318,22 +1388,25 @@
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="105">
+    <row r="6" spans="1:8" ht="105">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1341,22 +1414,25 @@
         <v>107</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1364,22 +1440,25 @@
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1387,22 +1466,25 @@
         <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1410,22 +1492,25 @@
         <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1433,22 +1518,25 @@
         <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1456,22 +1544,25 @@
         <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1479,22 +1570,25 @@
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1502,22 +1596,25 @@
         <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
@@ -1525,22 +1622,25 @@
         <v>103</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:8" ht="30">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1548,22 +1648,25 @@
         <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45">
+    <row r="16" spans="1:8" ht="45">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1571,22 +1674,25 @@
         <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1594,22 +1700,25 @@
         <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:8" ht="30">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1617,22 +1726,25 @@
         <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1640,22 +1752,25 @@
         <v>81</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45">
+    <row r="20" spans="1:8" ht="45">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1663,22 +1778,25 @@
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1686,22 +1804,25 @@
         <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1709,22 +1830,25 @@
         <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>109</v>
       </c>
@@ -1732,22 +1856,25 @@
         <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="225">
+    <row r="24" spans="1:8" ht="225">
       <c r="A24" s="2" t="s">
         <v>112</v>
       </c>
@@ -1755,22 +1882,25 @@
         <v>158</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="135">
+    <row r="25" spans="1:8" ht="135">
       <c r="A25" s="2" t="s">
         <v>114</v>
       </c>
@@ -1778,22 +1908,25 @@
         <v>134</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="135">
+    <row r="26" spans="1:8" ht="135">
       <c r="A26" s="2" t="s">
         <v>133</v>
       </c>
@@ -1801,22 +1934,25 @@
         <v>135</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="105">
+    <row r="27" spans="1:8" ht="105">
       <c r="A27" s="2" t="s">
         <v>116</v>
       </c>
@@ -1824,22 +1960,25 @@
         <v>162</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="105">
+    <row r="28" spans="1:8" ht="105">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -1847,22 +1986,25 @@
         <v>168</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="75">
+    <row r="29" spans="1:8" ht="75">
       <c r="A29" s="2" t="s">
         <v>115</v>
       </c>
@@ -1870,22 +2012,25 @@
         <v>131</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
         <v>118</v>
       </c>
@@ -1893,22 +2038,25 @@
         <v>121</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>119</v>
       </c>
@@ -1916,22 +2064,25 @@
         <v>122</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="75">
+    <row r="32" spans="1:8" ht="75">
       <c r="A32" s="2" t="s">
         <v>113</v>
       </c>
@@ -1939,22 +2090,25 @@
         <v>124</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
         <v>146</v>
       </c>
@@ -1962,22 +2116,25 @@
         <v>150</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
         <v>147</v>
       </c>
@@ -1985,22 +2142,25 @@
         <v>151</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
         <v>148</v>
       </c>
@@ -2008,22 +2168,25 @@
         <v>152</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
         <v>149</v>
       </c>
@@ -2031,18 +2194,21 @@
         <v>153</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="E36" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>212</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added simplified Chinese version (zh_cn)
</commit_message>
<xml_diff>
--- a/data_raw/EDT_dict.xlsx
+++ b/data_raw/EDT_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\EDT\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1056DFA-A176-4A7D-98DC-851D6D011158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAE5F78-2186-47F2-B7CA-4064616779AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDT" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="289">
   <si>
     <t>key</t>
   </si>
@@ -784,13 +784,146 @@
   </si>
   <si>
     <t>Nun geht es mit dem Haupttest los, in dem Ihre Ergebnisse gespeichert werden. \\ Ab jetzt bekommen Sie keine Rückmeldung mehr. Viel Erfolg!</t>
+  </si>
+  <si>
+    <t>欢迎参加情绪辨别测试</t>
+  </si>
+  <si>
+    <t>你将会听到一个旋律的两个不同版本；这两段旋律在情绪表达上有所不同。你的任务是判断每段旋律的情绪表达，从两段旋律中选择你认为最能代表问题中给出情绪的一段。 \\ 问题可能会重复出现，所以请不要担心作出两次相同的选择。请完整的听完每个片段，再作出决定。如果你不知道答案，请选择你的最佳猜测。</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题 {{num_question}} 用时 {{test_length}}</t>
+  </si>
+  <si>
+    <t>你的浏览器不支持此音频。如果没有音频支持，本测试将无法进行，抱歉！</t>
+  </si>
+  <si>
+    <t>请听下面的旋律，选择一个听起来**{{emotion}}**的片段。若选择哔声之前听到的旋律片段，则点击1；若选择哔声之后听到的片段，则点击2。</t>
+  </si>
+  <si>
+    <t>请选择一个选项</t>
+  </si>
+  <si>
+    <t>恭喜！</t>
+  </si>
+  <si>
+    <t>你正确识别了**{{accuracy}} %**的情绪。</t>
+  </si>
+  <si>
+    <t>更愤怒</t>
+  </si>
+  <si>
+    <t>更快乐</t>
+  </si>
+  <si>
+    <t>更温柔</t>
+  </si>
+  <si>
+    <t>更悲伤</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>更恐惧</t>
+  </si>
+  <si>
+    <t>请输入你的用户名</t>
+  </si>
+  <si>
+    <t>此用户名无效。请重试。</t>
+  </si>
+  <si>
+    <t>继续</t>
+  </si>
+  <si>
+    <t>你已完成情绪辨别测试。</t>
+  </si>
+  <si>
+    <t>情绪辨别测试</t>
+  </si>
+  <si>
+    <t>在{{num_question}}个问题中，你正确回答了{{num_correct}}个问题</t>
+  </si>
+  <si>
+    <t>你的分数</t>
+  </si>
+  <si>
+    <t>分数</t>
+  </si>
+  <si>
+    <t>返回</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;h4&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>欢迎参加音乐情绪辨别测试的训练&lt;/h4&gt; 你将被要求听几对预先录制的旋律，每个旋律表达了五种情绪类型中的一种：愤怒、恐惧、快乐、悲伤或温柔。你的任务是分辨每个音乐片段表达的情绪。 \\ 首先，你将听到几个例子，并做一些练习。</t>
+    </r>
+  </si>
+  <si>
+    <t>每个题目中你都会听到两段相似的旋律，但是它们有不同的情绪表达。点击播放聆听下面的片段，并决定两个旋律中哪一个听起来 **更快乐**。</t>
+  </si>
+  <si>
+    <t>这个例子中，表演者试图在哔声之前的旋律中表达快乐，在哔声之后的旋律中表达悲伤。所以正确的答案为片段1。你可以在继续之前再听一遍。</t>
+  </si>
+  <si>
+    <r>
+      <t>**练习 1** \\ 请听下面的旋律，选择听</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF434343"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>起来**更愤怒**的片段。 \\ 若选择哔声之前听到的旋律片段，则点击1；若选择哔声之后听到的片段，则点击2。</t>
+    </r>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ **练习 2** \\请听下面的旋律，选择听起来**更悲伤**的片段。 \\ 若选择哔声之前听到的旋律片段，则点击1；若选择哔声之后听到的片段，则点击2。</t>
+  </si>
+  <si>
+    <t>**{{feedback}}** \\ 点击“返回”，重新阅读指令并再次进行练习。或者点击“继续”，开始正式测试。</t>
+  </si>
+  <si>
+    <t>错误</t>
+  </si>
+  <si>
+    <t>正确！</t>
+  </si>
+  <si>
+    <t>现在开始正式测试，你的答案将被记录。 \\ 单个问题后不会收到反馈。祝你好运！</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>最愤怒</t>
+  </si>
+  <si>
+    <t>最快乐</t>
+  </si>
+  <si>
+    <t>最悲伤</t>
+  </si>
+  <si>
+    <t>最恐惧</t>
+  </si>
+  <si>
+    <t>ZH_CN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -836,6 +969,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF434343"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -857,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -883,6 +1034,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -939,7 +1092,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1258,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1276,7 +1429,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:9" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1301,8 +1454,11 @@
       <c r="H1" s="2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="30">
+      <c r="I1" s="9" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1327,8 +1483,11 @@
       <c r="H2" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="270">
+      <c r="I2" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="270">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1353,8 +1512,11 @@
       <c r="H3" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="31.5">
+      <c r="I3" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.5">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1379,8 +1541,11 @@
       <c r="H4" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="45">
+      <c r="I4" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1405,8 +1570,11 @@
       <c r="H5" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="105">
+      <c r="I5" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1431,8 +1599,11 @@
       <c r="H6" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1457,8 +1628,11 @@
       <c r="H7" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1483,8 +1657,11 @@
       <c r="H8" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="30">
+      <c r="I8" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1509,8 +1686,11 @@
       <c r="H9" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1535,8 +1715,11 @@
       <c r="H10" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1561,8 +1744,11 @@
       <c r="H11" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1587,8 +1773,11 @@
       <c r="H12" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1613,8 +1802,11 @@
       <c r="H13" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
@@ -1639,8 +1831,11 @@
       <c r="H14" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="30">
+      <c r="I14" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
@@ -1665,8 +1860,11 @@
       <c r="H15" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="45">
+      <c r="I15" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1691,8 +1889,11 @@
       <c r="H16" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1717,8 +1918,11 @@
       <c r="H17" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="30">
+      <c r="I17" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1743,8 +1947,11 @@
       <c r="H18" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1769,8 +1976,11 @@
       <c r="H19" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="45">
+      <c r="I19" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1795,8 +2005,11 @@
       <c r="H20" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1821,8 +2034,11 @@
       <c r="H21" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1847,8 +2063,11 @@
       <c r="H22" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
         <v>109</v>
       </c>
@@ -1873,8 +2092,11 @@
       <c r="H23" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="225">
+      <c r="I23" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="225">
       <c r="A24" s="2" t="s">
         <v>112</v>
       </c>
@@ -1899,8 +2121,11 @@
       <c r="H24" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="135">
+      <c r="I24" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="135">
       <c r="A25" s="2" t="s">
         <v>114</v>
       </c>
@@ -1925,8 +2150,11 @@
       <c r="H25" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="135">
+      <c r="I25" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="135">
       <c r="A26" s="2" t="s">
         <v>133</v>
       </c>
@@ -1951,8 +2179,11 @@
       <c r="H26" s="2" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="105">
+      <c r="I26" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="105">
       <c r="A27" s="2" t="s">
         <v>116</v>
       </c>
@@ -1977,8 +2208,11 @@
       <c r="H27" s="2" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="105">
+      <c r="I27" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="105">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -2003,8 +2237,11 @@
       <c r="H28" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="75">
+      <c r="I28" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="75">
       <c r="A29" s="2" t="s">
         <v>115</v>
       </c>
@@ -2029,8 +2266,11 @@
       <c r="H29" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
         <v>118</v>
       </c>
@@ -2055,8 +2295,11 @@
       <c r="H30" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
         <v>119</v>
       </c>
@@ -2081,8 +2324,11 @@
       <c r="H31" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="75">
+      <c r="I31" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="75">
       <c r="A32" s="2" t="s">
         <v>113</v>
       </c>
@@ -2107,8 +2353,11 @@
       <c r="H32" s="2" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
         <v>146</v>
       </c>
@@ -2133,8 +2382,11 @@
       <c r="H33" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
         <v>147</v>
       </c>
@@ -2159,8 +2411,11 @@
       <c r="H34" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" s="9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
         <v>148</v>
       </c>
@@ -2185,8 +2440,11 @@
       <c r="H35" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" s="9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
         <v>149</v>
       </c>
@@ -2210,6 +2468,9 @@
       </c>
       <c r="H36" s="2" t="s">
         <v>212</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>